<commit_message>
modified code to access webElement from different class
</commit_message>
<xml_diff>
--- a/TestData/OrangeHRMTestData.xlsx
+++ b/TestData/OrangeHRMTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minal\git\repository2\OrangeHRMtest\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D1D032-0FD7-46BA-B3E1-ABDCFC92EB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4C7AC5-BD99-4FCC-B098-7388A4EB1A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>minal</t>
+  </si>
+  <si>
+    <t>hghgbvc</t>
   </si>
 </sst>
 </file>
@@ -354,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -378,6 +384,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>